<commit_message>
Pre-AGU update for 2025
Contains all changes to code used to support the 2025 AGU poster along with new 5 micron data from Glenn
</commit_message>
<xml_diff>
--- a/Studies/NEZ/2024-2025 Mean Sys1 0-360 15N-15S blobs fNH3 Tracker.xlsx
+++ b/Studies/NEZ/2024-2025 Mean Sys1 0-360 15N-15S blobs fNH3 Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\Studies\NEZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12684492-98D5-4285-8EDD-4CB57B97176A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0D5262-0E98-4AA3-B056-C7A4591DB916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{62111891-02B3-4A17-BBDC-3BA2A745EE81}"/>
   </bookViews>
@@ -333,9 +333,6 @@
     <t>2024-11-29T07:32:24.429</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -427,6 +424,9 @@
   </si>
   <si>
     <t>2024-10-09T12:02:09.000</t>
+  </si>
+  <si>
+    <t>9?</t>
   </si>
 </sst>
 </file>
@@ -2884,10 +2884,10 @@
   <dimension ref="A1:T115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2952,16 +2952,16 @@
         <v>14</v>
       </c>
       <c r="Q1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" t="s">
         <v>100</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>101</v>
       </c>
-      <c r="S1" t="s">
-        <v>102</v>
-      </c>
       <c r="T1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
@@ -2972,7 +2972,7 @@
         <v>2460590.5920833298</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E2">
         <v>7</v>
@@ -3019,7 +3019,7 @@
         <v>2460593.9937499999</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3066,7 +3066,7 @@
         <v>2460593.9937499999</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -3116,7 +3116,7 @@
         <v>2460591.9952777699</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E5">
         <v>96</v>
@@ -3163,7 +3163,7 @@
         <v>2460592.0037500001</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3210,7 +3210,7 @@
         <v>2460592.0037500001</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -3257,7 +3257,7 @@
         <v>2460592.0037500001</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3351,7 +3351,7 @@
         <v>2460592.9932638798</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E10">
         <v>174</v>
@@ -3398,7 +3398,7 @@
         <v>2460593.0014930498</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -3445,7 +3445,7 @@
         <v>2460593.0014930498</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3492,7 +3492,7 @@
         <v>2460593.0014930498</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E13">
         <v>173</v>
@@ -3542,7 +3542,7 @@
         <v>2460619.7152972198</v>
       </c>
       <c r="D14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E14">
         <v>48</v>
@@ -3602,7 +3602,7 @@
         <v>2460619.7170138801</v>
       </c>
       <c r="D15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -3661,7 +3661,7 @@
         <v>2460619.7599305501</v>
       </c>
       <c r="D16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E16">
         <v>67</v>
@@ -3720,7 +3720,7 @@
         <v>2460619.8136111102</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17">
         <v>29</v>
@@ -3776,7 +3776,7 @@
         <v>2460619.82435185</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -3832,7 +3832,7 @@
         <v>2460619.8350868002</v>
       </c>
       <c r="D19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -3888,7 +3888,7 @@
         <v>2460619.8350868002</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -3944,7 +3944,7 @@
         <v>2460619.8360079299</v>
       </c>
       <c r="D21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E21">
         <v>8</v>
@@ -4003,7 +4003,7 @@
         <v>2460619.8594886302</v>
       </c>
       <c r="D22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E22">
         <v>5</v>
@@ -4059,7 +4059,7 @@
         <v>2460619.8887499999</v>
       </c>
       <c r="D23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E23">
         <v>404</v>
@@ -4115,7 +4115,7 @@
         <v>2460629.6912500001</v>
       </c>
       <c r="D24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E24">
         <v>96</v>
@@ -4165,7 +4165,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -4174,7 +4174,7 @@
         <v>2460629.75230555</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25">
         <v>290</v>
@@ -4230,7 +4230,7 @@
         <v>2460629.8124305499</v>
       </c>
       <c r="D26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E26">
         <v>323</v>
@@ -4289,7 +4289,7 @@
         <v>2460632.8283611098</v>
       </c>
       <c r="D27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E27">
         <v>266</v>
@@ -4349,7 +4349,7 @@
         <v>2460632.8428935101</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E28">
         <v>5</v>
@@ -4405,7 +4405,7 @@
         <v>2460632.8574305498</v>
       </c>
       <c r="D29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -4461,7 +4461,7 @@
         <v>2460632.6515509202</v>
       </c>
       <c r="D30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E30">
         <v>165</v>
@@ -4520,7 +4520,7 @@
         <v>2460632.6961388802</v>
       </c>
       <c r="D31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E31">
         <v>38</v>
@@ -4569,8 +4569,8 @@
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>9</v>
+      <c r="A32" t="s">
+        <v>129</v>
       </c>
       <c r="B32">
         <v>6</v>
@@ -4579,7 +4579,7 @@
         <v>2460632.7484722198</v>
       </c>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E32">
         <v>42</v>
@@ -4635,7 +4635,7 @@
         <v>2460632.76498737</v>
       </c>
       <c r="D33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -4967,8 +4967,8 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>98</v>
+      <c r="A39">
+        <v>7</v>
       </c>
       <c r="B39">
         <v>6</v>
@@ -5027,7 +5027,7 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40">
         <v>7</v>
@@ -5200,8 +5200,8 @@
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>9</v>
+      <c r="A43" t="s">
+        <v>129</v>
       </c>
       <c r="B43">
         <v>10</v>
@@ -5519,8 +5519,8 @@
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>98</v>
+      <c r="A49">
+        <v>7</v>
       </c>
       <c r="B49">
         <v>6</v>
@@ -5570,7 +5570,7 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50">
         <v>7</v>
@@ -8879,6 +8879,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:T115" xr:uid="{D98CA767-4D32-424D-86B7-C918E9E516BC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>